<commit_message>
Add the operation 'Reordering records' in all pertinent files. Modify 'Syntatic profiling' comment on the table
</commit_message>
<xml_diff>
--- a/data/data_wrangling.xlsx
+++ b/data/data_wrangling.xlsx
@@ -15,15 +15,15 @@
     <sheet name="data_wrangling_links_one_flow" sheetId="20" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">data_wrangling_links_one_flow!$A$1:$C$61</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$1:$G$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">data_wrangling_links_one_flow!$A$1:$C$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$1:$G$65</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="203">
   <si>
     <t>Data stage</t>
   </si>
@@ -469,9 +469,6 @@
     <t>Profiling for syntactic constraints involves simply checking whether data values are in (or not in) the set of permissible values.</t>
   </si>
   <si>
-    <t>Syntax refers to constraints on the literal values that are valid in a field (i.e., formatting).</t>
-  </si>
-  <si>
     <t>Profiling for semantic constraints involves checking whether data value meanings are in (or not in) the set of meaningful values.</t>
   </si>
   <si>
@@ -626,6 +623,15 @@
   </si>
   <si>
     <t>Act of changing the form or schema of the data.</t>
+  </si>
+  <si>
+    <t>Reordering records</t>
+  </si>
+  <si>
+    <t>Act of changing the order of records in the dataset.</t>
+  </si>
+  <si>
+    <t>Syntax refers to constraints on the literal values that are valid in a field (i.e., formatting or data types).</t>
   </si>
 </sst>
 </file>
@@ -992,7 +998,7 @@
   <sheetPr codeName="Plan1">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1010,7 +1016,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>97</v>
@@ -1019,7 +1025,7 @@
         <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>85</v>
@@ -1108,7 +1114,7 @@
         <v>87</v>
       </c>
       <c r="F5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G5" t="s">
         <v>119</v>
@@ -1131,7 +1137,7 @@
         <v>87</v>
       </c>
       <c r="F6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G6" t="s">
         <v>84</v>
@@ -1154,7 +1160,7 @@
         <v>87</v>
       </c>
       <c r="F7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G7" t="s">
         <v>120</v>
@@ -1243,7 +1249,7 @@
         <v>88</v>
       </c>
       <c r="F11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G11" t="s">
         <v>98</v>
@@ -1266,7 +1272,7 @@
         <v>88</v>
       </c>
       <c r="F12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G12" t="s">
         <v>99</v>
@@ -1289,7 +1295,7 @@
         <v>88</v>
       </c>
       <c r="F13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G13" t="s">
         <v>133</v>
@@ -1312,7 +1318,7 @@
         <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G14" t="s">
         <v>134</v>
@@ -1335,7 +1341,7 @@
         <v>88</v>
       </c>
       <c r="F15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G15" t="s">
         <v>56</v>
@@ -1358,7 +1364,7 @@
         <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G16" t="s">
         <v>53</v>
@@ -1742,7 +1748,7 @@
         <v>20</v>
       </c>
       <c r="F34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1762,7 +1768,7 @@
         <v>20</v>
       </c>
       <c r="F35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1782,7 +1788,7 @@
         <v>20</v>
       </c>
       <c r="F36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1802,7 +1808,7 @@
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G37" t="s">
         <v>95</v>
@@ -1825,7 +1831,7 @@
         <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1848,7 +1854,7 @@
         <v>147</v>
       </c>
       <c r="G39" t="s">
-        <v>148</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1868,7 +1874,7 @@
         <v>63</v>
       </c>
       <c r="F40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G40" t="s">
         <v>96</v>
@@ -1891,7 +1897,7 @@
         <v>63</v>
       </c>
       <c r="F41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1911,7 +1917,7 @@
         <v>63</v>
       </c>
       <c r="F42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -1931,7 +1937,7 @@
         <v>63</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1951,7 +1957,7 @@
         <v>63</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1971,10 +1977,10 @@
         <v>63</v>
       </c>
       <c r="F45" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G45" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1994,10 +2000,10 @@
         <v>63</v>
       </c>
       <c r="F46" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -2017,7 +2023,7 @@
         <v>63</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2037,10 +2043,10 @@
         <v>63</v>
       </c>
       <c r="F48" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G48" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2060,10 +2066,10 @@
         <v>71</v>
       </c>
       <c r="F49" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G49" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2083,7 +2089,7 @@
         <v>71</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2103,7 +2109,7 @@
         <v>71</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2123,7 +2129,7 @@
         <v>71</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2143,10 +2149,10 @@
         <v>71</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2166,7 +2172,7 @@
         <v>71</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2177,16 +2183,16 @@
         <v>16</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2197,19 +2203,16 @@
         <v>16</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="G56" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2220,16 +2223,19 @@
         <v>16</v>
       </c>
       <c r="C57" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
+      </c>
+      <c r="G57" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2240,19 +2246,16 @@
         <v>16</v>
       </c>
       <c r="C58" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2263,19 +2266,19 @@
         <v>16</v>
       </c>
       <c r="C59" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2286,19 +2289,19 @@
         <v>16</v>
       </c>
       <c r="C60" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E60" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -2309,16 +2312,19 @@
         <v>16</v>
       </c>
       <c r="C61" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>185</v>
+        <v>196</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -2329,16 +2335,16 @@
         <v>16</v>
       </c>
       <c r="C62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E62" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -2349,19 +2355,16 @@
         <v>16</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="G63" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -2372,32 +2375,55 @@
         <v>16</v>
       </c>
       <c r="C64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E64" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F64" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G64" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" t="s">
+        <v>73</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G65" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="G64" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D69" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -2704,7 +2730,7 @@
   <sheetPr codeName="Plan3">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3022,12 +3048,14 @@
         <v>25</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3041,7 +3069,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -3057,7 +3085,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -3073,7 +3101,7 @@
         <v>18</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -3086,14 +3114,12 @@
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3110,7 +3136,7 @@
         <v>45</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F23" s="3"/>
     </row>
@@ -3128,7 +3154,7 @@
         <v>45</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -3143,10 +3169,10 @@
         <v>44</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="F25" s="3"/>
     </row>
@@ -3164,7 +3190,7 @@
         <v>46</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F26" s="3"/>
     </row>
@@ -3182,7 +3208,7 @@
         <v>46</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="F27" s="3"/>
     </row>
@@ -3191,12 +3217,30 @@
         <v>16</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -3627,7 +3671,7 @@
   <sheetPr codeName="Plan5">
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3701,7 +3745,7 @@
         <v>25</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3860,10 +3904,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -3874,7 +3918,7 @@
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3885,7 +3929,7 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3893,10 +3937,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3907,7 +3951,7 @@
         <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3918,7 +3962,7 @@
         <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -3926,10 +3970,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -3940,7 +3984,7 @@
         <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -3948,13 +3992,13 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3962,7 +4006,7 @@
         <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>5</v>
@@ -3970,13 +4014,13 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3984,7 +4028,7 @@
         <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3995,7 +4039,7 @@
         <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -4006,7 +4050,7 @@
         <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -4014,13 +4058,13 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -4028,7 +4072,7 @@
         <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36">
         <v>3</v>
@@ -4036,13 +4080,13 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -4050,21 +4094,21 @@
         <v>26</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C39">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -4072,10 +4116,10 @@
         <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C40">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -4083,9 +4127,20 @@
         <v>25</v>
       </c>
       <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
         <v>44</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <v>6</v>
       </c>
     </row>
@@ -4100,7 +4155,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4365,10 +4420,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="C24" s="3">
         <v>0.5</v>
@@ -4379,7 +4434,7 @@
         <v>107</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C25" s="3">
         <v>0.5</v>
@@ -4390,7 +4445,7 @@
         <v>107</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="C26" s="3">
         <v>0.5</v>
@@ -4398,10 +4453,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C27" s="3">
         <v>0.5</v>
@@ -4412,7 +4467,7 @@
         <v>106</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C28" s="3">
         <v>0.5</v>
@@ -4423,21 +4478,21 @@
         <v>106</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="C29" s="3">
         <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" t="s">
-        <v>102</v>
+      <c r="A30" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="C30" s="3">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -4445,7 +4500,7 @@
         <v>112</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" s="3">
         <v>3</v>
@@ -4453,13 +4508,13 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>112</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C32" s="3">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -4467,7 +4522,7 @@
         <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C33" s="3">
         <v>2.5</v>
@@ -4475,13 +4530,13 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="C34" s="3">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -4489,7 +4544,7 @@
         <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" s="3">
         <v>0.5</v>
@@ -4500,7 +4555,7 @@
         <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" s="3">
         <v>0.5</v>
@@ -4511,7 +4566,7 @@
         <v>18</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="3">
         <v>0.5</v>
@@ -4519,13 +4574,13 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>107</v>
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
       </c>
       <c r="C38" s="3">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -4533,21 +4588,21 @@
         <v>44</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C39" s="3">
         <v>1.5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>26</v>
+      <c r="A40" t="s">
+        <v>44</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C40" s="3">
-        <v>6</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -4555,21 +4610,21 @@
         <v>26</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C41" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="C42" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -4577,10 +4632,10 @@
         <v>25</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C43" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -4588,26 +4643,26 @@
         <v>25</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C45" s="3">
         <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>114</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="3">
-        <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>17</v>
@@ -4618,7 +4673,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>17</v>
@@ -4629,7 +4684,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>17</v>
@@ -4640,7 +4695,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>17</v>
@@ -4651,7 +4706,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>17</v>
@@ -4662,7 +4717,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>17</v>
@@ -4673,7 +4728,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>17</v>
@@ -4684,7 +4739,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>17</v>
@@ -4695,7 +4750,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>17</v>
@@ -4706,7 +4761,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>17</v>
@@ -4717,7 +4772,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>17</v>
@@ -4728,7 +4783,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>17</v>
@@ -4739,7 +4794,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>17</v>
@@ -4749,19 +4804,19 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>64</v>
+      <c r="A59" t="s">
+        <v>43</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C59" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>17</v>
@@ -4772,7 +4827,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>17</v>
@@ -4782,9 +4837,20 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
+      <c r="A62" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>